<commit_message>
Attendance reading from excel file completed
Config changed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Settings" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Constants" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Assets" sheetId="3" r:id="rId5"/>
+    <sheet name="Settings" sheetId="1" r:id="rId1"/>
+    <sheet name="Constants" sheetId="2" r:id="rId2"/>
+    <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -21,162 +29,218 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>MaxRetryNumber</t>
+  </si>
+  <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with application exception. Must be integer</t>
+  </si>
+  <si>
+    <t>TimeoutShort</t>
+  </si>
+  <si>
+    <t>Timeout short value in milliseconds, for activities which are likely to fail. Must be integer</t>
+  </si>
+  <si>
+    <t>TimeoutMedium</t>
+  </si>
+  <si>
+    <t>Timeout medium value in milliseconds. Must be integer</t>
+  </si>
+  <si>
+    <t>TimeoutLong</t>
+  </si>
+  <si>
+    <t>Timeout short value in milliseconds, for slow apps. Must be integer</t>
+  </si>
+  <si>
+    <t>ExScreenshotsFolderPath</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
+  </si>
+  <si>
+    <t>DelayShort</t>
+  </si>
+  <si>
+    <t>Delay short value in milliseconds, for activities where it is necessary to wait a little. Must be integer</t>
+  </si>
+  <si>
+    <t>DelayMedium</t>
+  </si>
+  <si>
+    <t>Delay medium value in milliseconds, for activities where it is necessary to wait a moderate amount of time. Must be integer</t>
+  </si>
+  <si>
+    <t>DelayLong</t>
+  </si>
+  <si>
+    <t>Delay long value in milliseconds, for activities where it is necessary to wait a long time. Must be integer</t>
+  </si>
+  <si>
+    <t>AccuracyLow</t>
+  </si>
+  <si>
+    <t>Image accuracy low value, for images that have high contrast. Must be double</t>
+  </si>
+  <si>
+    <t>AccuracyMedium</t>
+  </si>
+  <si>
+    <t>Image accuracy medium value, for images that have normal contrast. Must be double</t>
+  </si>
+  <si>
+    <t>AccuracyHigh</t>
+  </si>
+  <si>
+    <t>Image accuracy high value, for images that have low contrast. Must be double</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionDataError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Error retrieving Transaction Data.</t>
+  </si>
+  <si>
+    <t>LogMessage_Success</t>
+  </si>
+  <si>
+    <t>Transaction Successful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful</t>
+  </si>
+  <si>
+    <t>LogMessage_BusinessRuleException</t>
+  </si>
+  <si>
+    <t>Business rule exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception</t>
+  </si>
+  <si>
+    <t>LogMessage_ApplicationException</t>
+  </si>
+  <si>
+    <t>System exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception</t>
+  </si>
+  <si>
     <t>Asset</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Description (Assets will always overwrite other config)</t>
   </si>
   <si>
-    <t>MaxRetryNumber</t>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with application exception. Must be integer</t>
-  </si>
-  <si>
-    <t>TimeoutShort</t>
-  </si>
-  <si>
-    <t>Timeout short value in milliseconds, for activities which are likely to fail. Must be integer</t>
-  </si>
-  <si>
-    <t>TimeoutMedium</t>
-  </si>
-  <si>
-    <t>Timeout medium value in milliseconds. Must be integer</t>
-  </si>
-  <si>
-    <t>TimeoutLong</t>
-  </si>
-  <si>
-    <t>Timeout short value in milliseconds, for slow apps. Must be integer</t>
-  </si>
-  <si>
-    <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
-    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
-  </si>
-  <si>
-    <t>DelayShort</t>
-  </si>
-  <si>
-    <t>Delay short value in milliseconds, for activities where it is necessary to wait a little. Must be integer</t>
-  </si>
-  <si>
-    <t>DelayMedium</t>
-  </si>
-  <si>
-    <t>Delay medium value in milliseconds, for activities where it is necessary to wait a moderate amount of time. Must be integer</t>
-  </si>
-  <si>
-    <t>DelayLong</t>
-  </si>
-  <si>
-    <t>Delay long value in milliseconds, for activities where it is necessary to wait a long time. Must be integer</t>
-  </si>
-  <si>
-    <t>AccuracyLow</t>
-  </si>
-  <si>
-    <t>Image accuracy low value, for images that have high contrast. Must be double</t>
-  </si>
-  <si>
-    <t>AccuracyMedium</t>
-  </si>
-  <si>
-    <t>Image accuracy medium value, for images that have normal contrast. Must be double</t>
-  </si>
-  <si>
-    <t>AccuracyHigh</t>
-  </si>
-  <si>
-    <t>Image accuracy high value, for images that have low contrast. Must be double</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processing Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionDataError</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Error retrieving Transaction Data.</t>
-  </si>
-  <si>
-    <t>LogMessage_Success</t>
-  </si>
-  <si>
-    <t>Transaction Successful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful</t>
-  </si>
-  <si>
-    <t>LogMessage_BusinessRuleException</t>
-  </si>
-  <si>
-    <t>Business rule exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception</t>
-  </si>
-  <si>
-    <t>LogMessage_ApplicationException</t>
-  </si>
-  <si>
-    <t>System exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-  </si>
-  <si>
-    <t>KibanaDemoQueue</t>
-  </si>
-  <si>
-    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
-  </si>
-  <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
+    <t>Attendance Format</t>
+  </si>
+  <si>
+    <t>Attendance Threshold</t>
+  </si>
+  <si>
+    <t>Input Directory</t>
+  </si>
+  <si>
+    <t>C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\Input</t>
+  </si>
+  <si>
+    <t>Output Directory</t>
+  </si>
+  <si>
+    <t>C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\Output</t>
+  </si>
+  <si>
+    <t>Number_Batches</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>SUAS</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>Attendance Column Fields</t>
+  </si>
+  <si>
+    <t>Number Sessions Cell</t>
+  </si>
+  <si>
+    <t>Headers Row</t>
+  </si>
+  <si>
+    <t>Column Names to fetch from attendance file</t>
+  </si>
+  <si>
+    <t>Row number containing column names</t>
+  </si>
+  <si>
+    <t>Start Date Column</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A:C</t>
+  </si>
+  <si>
+    <t>Subject Name Cell</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>Attendance Column Field Count</t>
+  </si>
+  <si>
+    <t>1/0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
-      <color rgb="FF000000"/>
+      <sz val="14"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,54 +248,392 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:satMod val="350000"/>
+                <a:shade val="99000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="_h" fmla="val 21600"/>
+            <a:gd name="_w" fmla="val 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600"/>
+          </a:pathLst>
+        </a:custGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="9CBEE0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="739CC3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="200000"/>
+        </a:ln>
+      </a:spPr>
+      <a:bodyPr/>
+      <a:lstStyle/>
+    </a:spDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="68.0"/>
-    <col customWidth="1" min="2" max="2" width="70.14"/>
-    <col customWidth="1" min="3" max="3" width="68.57"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col min="1" max="1" width="68" customWidth="1"/>
+    <col min="2" max="2" width="70.109375" customWidth="1"/>
+    <col min="3" max="3" width="68.5546875" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -239,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -265,41 +667,63 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
         <v>43</v>
       </c>
       <c r="B2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
         <v>45</v>
       </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1282,24 +1706,29 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="53.0"/>
-    <col customWidth="1" min="2" max="2" width="63.57"/>
-    <col customWidth="1" min="3" max="3" width="89.0"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="89" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1307,7 +1736,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1333,197 +1762,246 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>0.0</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B5">
+        <v>5000</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>5000.0</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6">
+        <v>30000</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>30000.0</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7">
+        <v>120000</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
-        <v>120000.0</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B11">
+        <v>1000</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <v>1000.0</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B12">
+        <v>15000</v>
+      </c>
+      <c r="C12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B12">
-        <v>15000.0</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B13">
+        <v>60000</v>
+      </c>
+      <c r="C13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
         <v>20</v>
-      </c>
-      <c r="B13">
-        <v>60000.0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>22</v>
       </c>
       <c r="B15">
         <v>0.6</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>0.8</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>0.9</v>
       </c>
       <c r="C17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
         <v>27</v>
       </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
         <v>30</v>
       </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B21" t="s">
         <v>33</v>
       </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B22" t="s">
         <v>36</v>
       </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B23" t="s">
         <v>39</v>
       </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2492,30 +2970,36 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="65.43"/>
+    <col min="1" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2541,21 +3025,21 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -3541,6 +4025,8 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Attendance sumary creation done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>1/0</t>
+  </si>
+  <si>
+    <t>Summary File Name</t>
+  </si>
+  <si>
+    <t>Summary.xlsx</t>
   </si>
 </sst>
 </file>
@@ -621,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1716,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2000,7 +2006,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Framework modified - activities added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -161,15 +161,9 @@
     <t>Input Directory</t>
   </si>
   <si>
-    <t>C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\Input</t>
-  </si>
-  <si>
     <t>Output Directory</t>
   </si>
   <si>
-    <t>C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\Output</t>
-  </si>
-  <si>
     <t>Number_Batches</t>
   </si>
   <si>
@@ -215,13 +209,28 @@
     <t>Attendance Column Field Count</t>
   </si>
   <si>
+    <t>Summary File Name</t>
+  </si>
+  <si>
+    <t>Summary.xlsx</t>
+  </si>
+  <si>
+    <t>Trnsaction Workbook Name</t>
+  </si>
+  <si>
+    <t>Transactions.xlsx</t>
+  </si>
+  <si>
+    <t>Name of workbook that stores all statuses of transaction</t>
+  </si>
+  <si>
+    <t>C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\Demo\Input</t>
+  </si>
+  <si>
+    <t>C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\Demo\Output</t>
+  </si>
+  <si>
     <t>1/0</t>
-  </si>
-  <si>
-    <t>Summary File Name</t>
-  </si>
-  <si>
-    <t>Summary.xlsx</t>
   </si>
 </sst>
 </file>
@@ -271,12 +280,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -627,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -677,8 +689,8 @@
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>64</v>
+      <c r="B2" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -694,31 +706,31 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1722,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1953,26 +1965,26 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2">
         <v>3</v>
@@ -1981,56 +1993,66 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28">
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
README added and minor bug fixes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -201,36 +201,6 @@
   </si>
   <si>
     <t>Name of workbook that stores all statuses of transaction</t>
-  </si>
-  <si>
-    <t>Attendance Format</t>
-  </si>
-  <si>
-    <t>1/0</t>
-  </si>
-  <si>
-    <t>Attendance Threshold</t>
-  </si>
-  <si>
-    <t>Input Directory</t>
-  </si>
-  <si>
-    <t>C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\Demo\Input</t>
-  </si>
-  <si>
-    <t>Output Directory</t>
-  </si>
-  <si>
-    <t>C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\Demo\Output</t>
-  </si>
-  <si>
-    <t>Number_Batches</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>SUAS</t>
   </si>
 </sst>
 </file>
@@ -640,7 +610,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -686,53 +656,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Sample attendance files added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAAE64C-97B5-4ABF-B17E-3FD7829CDEEA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -203,40 +204,13 @@
     <t>Name of workbook that stores all statuses of transaction</t>
   </si>
   <si>
-    <t>Attendance Format</t>
-  </si>
-  <si>
-    <t>1/0</t>
-  </si>
-  <si>
-    <t>Attendance Threshold</t>
-  </si>
-  <si>
-    <t>Input Directory</t>
-  </si>
-  <si>
-    <t>C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\Demo\Input</t>
-  </si>
-  <si>
-    <t>Output Directory</t>
-  </si>
-  <si>
-    <t>C:\Users\Samyak\Documents\UiPath\UiPath-Attendance-Framework-UAF\Data\Demo\Output</t>
-  </si>
-  <si>
-    <t>Number_Batches</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>SUAS</t>
+    <t>Number of columns as headers in attendance sheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -636,11 +610,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -686,53 +660,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1731,11 +1665,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1989,7 +1923,9 @@
       <c r="B27" s="2">
         <v>3</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="2" t="s">
@@ -3014,7 +2950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>